<commit_message>
moved NOACTION to actioncodes
</commit_message>
<xml_diff>
--- a/lizard_progress/util/tests/test_autoreviewer_files/filter_complete_valid.xlsx
+++ b/lizard_progress/util/tests/test_autoreviewer_files/filter_complete_valid.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="57">
   <si>
     <t xml:space="preserve">HCTag</t>
   </si>
@@ -61,7 +61,7 @@
     <t xml:space="preserve">&lt;D&gt; &lt;/D&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">&gt;5</t>
+    <t xml:space="preserve">&gt;=5</t>
   </si>
   <si>
     <t xml:space="preserve">&gt;=10</t>
@@ -115,7 +115,7 @@
     <t xml:space="preserve">BAG</t>
   </si>
   <si>
-    <t xml:space="preserve">&gt;25</t>
+    <t xml:space="preserve">&gt;=25</t>
   </si>
   <si>
     <t xml:space="preserve">BAH</t>
@@ -164,9 +164,6 @@
   </si>
   <si>
     <t xml:space="preserve">BBB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&gt;10</t>
   </si>
   <si>
     <t xml:space="preserve">BBC</t>
@@ -301,8 +298,8 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I23" activeCellId="0" sqref="I23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G29" activeCellId="0" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -652,11 +649,8 @@
       <c r="G22" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="I22" s="0" t="s">
-        <v>13</v>
-      </c>
       <c r="J22" s="1" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -664,13 +658,13 @@
         <v>10</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G23" s="0" t="s">
         <v>12</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -678,13 +672,13 @@
         <v>10</v>
       </c>
       <c r="B24" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I24" s="0" t="s">
         <v>50</v>
-      </c>
-      <c r="C24" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="I24" s="0" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -692,13 +686,13 @@
         <v>10</v>
       </c>
       <c r="B25" s="0" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="I25" s="0" t="s">
         <v>52</v>
-      </c>
-      <c r="C25" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="I25" s="0" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -706,7 +700,7 @@
         <v>10</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C26" s="0" t="s">
         <v>16</v>
@@ -715,7 +709,7 @@
         <v>26</v>
       </c>
       <c r="J26" s="0" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -723,7 +717,7 @@
         <v>10</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -731,7 +725,7 @@
         <v>10</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>